<commit_message>
Scraper works now with future matches
</commit_message>
<xml_diff>
--- a/bet365_odds.xlsx
+++ b/bet365_odds.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,55 +578,55 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Annecy</t>
+          <t>Gaziantep</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Troyes</t>
+          <t>Goztepe</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.73</v>
+        <v>2.35</v>
       </c>
       <c r="D2" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="E2" t="n">
-        <v>4.5</v>
+        <v>2.88</v>
       </c>
       <c r="F2" t="n">
-        <v>1.18</v>
+        <v>1.4</v>
       </c>
       <c r="G2" t="n">
         <v>1.29</v>
       </c>
       <c r="H2" t="n">
-        <v>2.05</v>
+        <v>1.57</v>
       </c>
       <c r="I2" t="n">
-        <v>2.38</v>
+        <v>3</v>
       </c>
       <c r="J2" t="n">
         <v>2.2</v>
       </c>
       <c r="K2" t="n">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="L2" t="n">
-        <v>1.17</v>
+        <v>1.29</v>
       </c>
       <c r="M2" t="n">
         <v>1.62</v>
       </c>
       <c r="N2" t="n">
-        <v>1.53</v>
+        <v>1.36</v>
       </c>
       <c r="O2" t="n">
-        <v>1.83</v>
+        <v>1.73</v>
       </c>
       <c r="P2" t="n">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="Q2" t="n">
         <v>1.29</v>
@@ -635,10 +635,10 @@
         <v>3.5</v>
       </c>
       <c r="S2" t="n">
-        <v>1.93</v>
+        <v>1.95</v>
       </c>
       <c r="T2" t="n">
-        <v>1.93</v>
+        <v>1.9</v>
       </c>
       <c r="U2" t="n">
         <v>3.25</v>
@@ -653,10 +653,10 @@
         <v>1.11</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.36</v>
+        <v>1.4</v>
       </c>
       <c r="Z2" t="n">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="AA2" t="n">
         <v>2.75</v>
@@ -668,55 +668,55 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Clermont</t>
+          <t>Ulm</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Red Star</t>
+          <t>Schalke</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.91</v>
+        <v>2.63</v>
       </c>
       <c r="D3" t="n">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="E3" t="n">
-        <v>3.9</v>
+        <v>2.63</v>
       </c>
       <c r="F3" t="n">
-        <v>1.25</v>
+        <v>1.44</v>
       </c>
       <c r="G3" t="n">
-        <v>1.29</v>
+        <v>1.33</v>
       </c>
       <c r="H3" t="n">
-        <v>1.83</v>
+        <v>1.44</v>
       </c>
       <c r="I3" t="n">
-        <v>2.6</v>
+        <v>3.25</v>
       </c>
       <c r="J3" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="K3" t="n">
-        <v>4.33</v>
+        <v>3.25</v>
       </c>
       <c r="L3" t="n">
-        <v>1.2</v>
+        <v>1.33</v>
       </c>
       <c r="M3" t="n">
-        <v>1.62</v>
+        <v>1.67</v>
       </c>
       <c r="N3" t="n">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
       <c r="O3" t="n">
-        <v>1.8</v>
+        <v>1.73</v>
       </c>
       <c r="P3" t="n">
-        <v>1.91</v>
+        <v>2</v>
       </c>
       <c r="Q3" t="n">
         <v>1.3</v>
@@ -725,10 +725,10 @@
         <v>3.4</v>
       </c>
       <c r="S3" t="n">
-        <v>2</v>
+        <v>2.03</v>
       </c>
       <c r="T3" t="n">
-        <v>1.85</v>
+        <v>1.83</v>
       </c>
       <c r="U3" t="n">
         <v>3.4</v>
@@ -758,217 +758,217 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Rodez</t>
+          <t>Preussen Munster</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Laval</t>
+          <t>Dusseldorf</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.2</v>
+        <v>3.2</v>
       </c>
       <c r="D4" t="n">
-        <v>3.25</v>
+        <v>3.6</v>
       </c>
       <c r="E4" t="n">
-        <v>3.25</v>
+        <v>2.15</v>
       </c>
       <c r="F4" t="n">
-        <v>1.33</v>
+        <v>1.67</v>
       </c>
       <c r="G4" t="n">
-        <v>1.33</v>
+        <v>1.29</v>
       </c>
       <c r="H4" t="n">
-        <v>1.67</v>
+        <v>1.36</v>
       </c>
       <c r="I4" t="n">
-        <v>2.88</v>
+        <v>3.5</v>
       </c>
       <c r="J4" t="n">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="K4" t="n">
-        <v>3.75</v>
+        <v>2.75</v>
       </c>
       <c r="L4" t="n">
-        <v>1.25</v>
+        <v>1.4</v>
       </c>
       <c r="M4" t="n">
-        <v>1.62</v>
+        <v>1.57</v>
       </c>
       <c r="N4" t="n">
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="O4" t="n">
-        <v>1.83</v>
+        <v>1.53</v>
       </c>
       <c r="P4" t="n">
-        <v>1.83</v>
+        <v>2.38</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.33</v>
+        <v>1.2</v>
       </c>
       <c r="R4" t="n">
-        <v>3.25</v>
+        <v>4.33</v>
       </c>
       <c r="S4" t="n">
-        <v>2.08</v>
+        <v>1.7</v>
       </c>
       <c r="T4" t="n">
-        <v>1.73</v>
+        <v>2.1</v>
       </c>
       <c r="U4" t="n">
-        <v>3.75</v>
+        <v>2.63</v>
       </c>
       <c r="V4" t="n">
-        <v>1.25</v>
+        <v>1.44</v>
       </c>
       <c r="W4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="X4" t="n">
-        <v>1.08</v>
+        <v>1.17</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.36</v>
+        <v>1.3</v>
       </c>
       <c r="Z4" t="n">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="AA4" t="n">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="AB4" t="n">
-        <v>1.4</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Metz</t>
+          <t>Monaco</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lorient</t>
+          <t>Angers</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.45</v>
+        <v>1.22</v>
       </c>
       <c r="D5" t="n">
-        <v>3.25</v>
+        <v>6.5</v>
       </c>
       <c r="E5" t="n">
-        <v>2.63</v>
+        <v>12</v>
       </c>
       <c r="F5" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="K5" t="n">
+        <v>9</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="M5" t="n">
         <v>1.4</v>
       </c>
-      <c r="G5" t="n">
+      <c r="N5" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="R5" t="n">
+        <v>6</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="T5" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="U5" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="V5" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="W5" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="X5" t="n">
         <v>1.3</v>
       </c>
-      <c r="H5" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="I5" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="J5" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="K5" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="M5" t="n">
-        <v>1.67</v>
-      </c>
-      <c r="N5" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="O5" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="P5" t="n">
-        <v>1.91</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="R5" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="S5" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="T5" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="U5" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="V5" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="W5" t="n">
-        <v>7</v>
-      </c>
-      <c r="X5" t="n">
-        <v>1.1</v>
-      </c>
       <c r="Y5" t="n">
-        <v>1.44</v>
+        <v>1.22</v>
       </c>
       <c r="Z5" t="n">
-        <v>2.63</v>
+        <v>4</v>
       </c>
       <c r="AA5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.36</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Amiens</t>
+          <t>Alverca</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Clermont</t>
+          <t>Feirense</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.4</v>
+        <v>2.25</v>
       </c>
       <c r="D6" t="n">
-        <v>2.9</v>
+        <v>3.25</v>
       </c>
       <c r="E6" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="I6" t="n">
         <v>3</v>
       </c>
-      <c r="F6" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3.25</v>
-      </c>
       <c r="J6" t="n">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="K6" t="n">
         <v>3.75</v>
@@ -977,238 +977,238 @@
         <v>1.25</v>
       </c>
       <c r="M6" t="n">
-        <v>1.8</v>
+        <v>1.73</v>
       </c>
       <c r="N6" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="R6" t="n">
+        <v>3</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="U6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="V6" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="W6" t="n">
+        <v>9</v>
+      </c>
+      <c r="X6" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="AB6" t="n">
         <v>1.33</v>
-      </c>
-      <c r="O6" t="n">
-        <v>2</v>
-      </c>
-      <c r="P6" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>1.44</v>
-      </c>
-      <c r="R6" t="n">
-        <v>2.63</v>
-      </c>
-      <c r="S6" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="T6" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="U6" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="V6" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="W6" t="n">
-        <v>11</v>
-      </c>
-      <c r="X6" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>2.38</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>1.29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bastia</t>
+          <t>Clermont</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Paris FC</t>
+          <t>Lorient</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>4.2</v>
       </c>
       <c r="D7" t="n">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="E7" t="n">
-        <v>2.38</v>
+        <v>1.85</v>
       </c>
       <c r="F7" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="I7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L7" t="n">
         <v>1.5</v>
       </c>
-      <c r="G7" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="H7" t="n">
+      <c r="M7" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="P7" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="R7" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="U7" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="V7" t="n">
         <v>1.33</v>
       </c>
-      <c r="I7" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="J7" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="M7" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="N7" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="O7" t="n">
-        <v>2</v>
-      </c>
-      <c r="P7" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>1.44</v>
-      </c>
-      <c r="R7" t="n">
-        <v>2.63</v>
-      </c>
-      <c r="S7" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="T7" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="U7" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="V7" t="n">
-        <v>1.18</v>
-      </c>
       <c r="W7" t="n">
-        <v>11</v>
+        <v>6.5</v>
       </c>
       <c r="X7" t="n">
-        <v>1.05</v>
+        <v>1.11</v>
       </c>
       <c r="Y7" t="n">
-        <v>1.5</v>
+        <v>1.37</v>
       </c>
       <c r="Z7" t="n">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="AA7" t="n">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="AB7" t="n">
-        <v>1.29</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Caen</t>
+          <t>Paris FC</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AC Ajaccio</t>
+          <t>Rodez</t>
         </is>
       </c>
       <c r="C8" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="K8" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="R8" t="n">
+        <v>4</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="T8" t="n">
         <v>2</v>
       </c>
-      <c r="D8" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1.67</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2.88</v>
-      </c>
-      <c r="J8" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1.17</v>
-      </c>
-      <c r="M8" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="N8" t="n">
+      <c r="U8" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="V8" t="n">
         <v>1.4</v>
       </c>
-      <c r="O8" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="P8" t="n">
-        <v>1.67</v>
-      </c>
-      <c r="Q8" t="n">
+      <c r="W8" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="X8" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="AB8" t="n">
         <v>1.44</v>
-      </c>
-      <c r="R8" t="n">
-        <v>2.63</v>
-      </c>
-      <c r="S8" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="T8" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="U8" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="V8" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="W8" t="n">
-        <v>11</v>
-      </c>
-      <c r="X8" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>2.38</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>1.29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dunkerque</t>
+          <t>Annecy</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1217,46 +1217,46 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="D9" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="E9" t="n">
         <v>3.1</v>
       </c>
-      <c r="E9" t="n">
-        <v>2.45</v>
-      </c>
       <c r="F9" t="n">
-        <v>1.53</v>
+        <v>1.36</v>
       </c>
       <c r="G9" t="n">
-        <v>1.36</v>
+        <v>1.33</v>
       </c>
       <c r="H9" t="n">
-        <v>1.4</v>
+        <v>1.62</v>
       </c>
       <c r="I9" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="J9" t="n">
-        <v>2.05</v>
+        <v>2.1</v>
       </c>
       <c r="K9" t="n">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="L9" t="n">
-        <v>1.36</v>
+        <v>1.29</v>
       </c>
       <c r="M9" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="O9" t="n">
         <v>1.73</v>
       </c>
-      <c r="N9" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="O9" t="n">
-        <v>1.83</v>
-      </c>
       <c r="P9" t="n">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="Q9" t="n">
         <v>1.3</v>
@@ -1265,10 +1265,10 @@
         <v>3.4</v>
       </c>
       <c r="S9" t="n">
-        <v>2.05</v>
+        <v>2.03</v>
       </c>
       <c r="T9" t="n">
-        <v>1.75</v>
+        <v>1.83</v>
       </c>
       <c r="U9" t="n">
         <v>3.5</v>
@@ -1283,64 +1283,64 @@
         <v>1.1</v>
       </c>
       <c r="Y9" t="n">
-        <v>1.44</v>
+        <v>1.4</v>
       </c>
       <c r="Z9" t="n">
-        <v>2.63</v>
+        <v>2.75</v>
       </c>
       <c r="AA9" t="n">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="AB9" t="n">
-        <v>1.33</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Guingamp</t>
+          <t>Dunkerque</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Annecy</t>
+          <t>Amiens</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.75</v>
+        <v>2.3</v>
       </c>
       <c r="D10" t="n">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="E10" t="n">
-        <v>4.33</v>
+        <v>3.1</v>
       </c>
       <c r="F10" t="n">
-        <v>1.18</v>
+        <v>1.36</v>
       </c>
       <c r="G10" t="n">
-        <v>1.29</v>
+        <v>1.36</v>
       </c>
       <c r="H10" t="n">
-        <v>1.91</v>
+        <v>1.57</v>
       </c>
       <c r="I10" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="J10" t="n">
-        <v>2.2</v>
+        <v>2.05</v>
       </c>
       <c r="K10" t="n">
-        <v>4.75</v>
+        <v>3.75</v>
       </c>
       <c r="L10" t="n">
-        <v>1.17</v>
+        <v>1.25</v>
       </c>
       <c r="M10" t="n">
-        <v>1.62</v>
+        <v>1.73</v>
       </c>
       <c r="N10" t="n">
-        <v>1.53</v>
+        <v>1.36</v>
       </c>
       <c r="O10" t="n">
         <v>1.83</v>
@@ -1349,40 +1349,40 @@
         <v>1.83</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.3</v>
+        <v>1.36</v>
       </c>
       <c r="R10" t="n">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="S10" t="n">
-        <v>2.03</v>
+        <v>2.15</v>
       </c>
       <c r="T10" t="n">
-        <v>1.83</v>
+        <v>1.67</v>
       </c>
       <c r="U10" t="n">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="V10" t="n">
-        <v>1.29</v>
+        <v>1.25</v>
       </c>
       <c r="W10" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="X10" t="n">
-        <v>1.1</v>
+        <v>1.07</v>
       </c>
       <c r="Y10" t="n">
-        <v>1.4</v>
+        <v>1.44</v>
       </c>
       <c r="Z10" t="n">
-        <v>2.75</v>
+        <v>2.63</v>
       </c>
       <c r="AA10" t="n">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="AB10" t="n">
-        <v>1.36</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="11">
@@ -1393,92 +1393,92 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Grenoble</t>
+          <t>Red Star</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="E11" t="n">
-        <v>2.35</v>
+        <v>2.15</v>
       </c>
       <c r="F11" t="n">
-        <v>1.57</v>
+        <v>1.67</v>
       </c>
       <c r="G11" t="n">
         <v>1.36</v>
       </c>
       <c r="H11" t="n">
-        <v>1.36</v>
+        <v>1.3</v>
       </c>
       <c r="I11" t="n">
         <v>4</v>
       </c>
       <c r="J11" t="n">
-        <v>1.91</v>
+        <v>2.1</v>
       </c>
       <c r="K11" t="n">
-        <v>3.25</v>
+        <v>2.88</v>
       </c>
       <c r="L11" t="n">
-        <v>1.33</v>
+        <v>1.4</v>
       </c>
       <c r="M11" t="n">
-        <v>1.8</v>
+        <v>1.67</v>
       </c>
       <c r="N11" t="n">
         <v>1.22</v>
       </c>
       <c r="O11" t="n">
-        <v>2.25</v>
+        <v>1.83</v>
       </c>
       <c r="P11" t="n">
-        <v>1.57</v>
+        <v>1.83</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.53</v>
+        <v>1.33</v>
       </c>
       <c r="R11" t="n">
-        <v>2.38</v>
+        <v>3.25</v>
       </c>
       <c r="S11" t="n">
-        <v>2.7</v>
+        <v>2.1</v>
       </c>
       <c r="T11" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="U11" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="V11" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="W11" t="n">
+        <v>8</v>
+      </c>
+      <c r="X11" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="Y11" t="n">
         <v>1.44</v>
       </c>
-      <c r="U11" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="V11" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="W11" t="n">
-        <v>13</v>
-      </c>
-      <c r="X11" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>1.62</v>
-      </c>
       <c r="Z11" t="n">
-        <v>2.2</v>
+        <v>2.63</v>
       </c>
       <c r="AA11" t="n">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="AB11" t="n">
-        <v>1.22</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Red Star</t>
+          <t>Troyes</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1487,46 +1487,46 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2.45</v>
+        <v>2.05</v>
       </c>
       <c r="D12" t="n">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="E12" t="n">
-        <v>2.8</v>
+        <v>3.7</v>
       </c>
       <c r="F12" t="n">
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="G12" t="n">
         <v>1.36</v>
       </c>
       <c r="H12" t="n">
-        <v>1.53</v>
+        <v>1.73</v>
       </c>
       <c r="I12" t="n">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="J12" t="n">
         <v>2.05</v>
       </c>
       <c r="K12" t="n">
-        <v>3.6</v>
+        <v>4.33</v>
       </c>
       <c r="L12" t="n">
-        <v>1.29</v>
+        <v>1.2</v>
       </c>
       <c r="M12" t="n">
         <v>1.73</v>
       </c>
       <c r="N12" t="n">
-        <v>1.33</v>
+        <v>1.4</v>
       </c>
       <c r="O12" t="n">
-        <v>1.83</v>
+        <v>1.91</v>
       </c>
       <c r="P12" t="n">
-        <v>1.83</v>
+        <v>1.8</v>
       </c>
       <c r="Q12" t="n">
         <v>1.36</v>
@@ -1553,106 +1553,826 @@
         <v>1.07</v>
       </c>
       <c r="Y12" t="n">
-        <v>1.5</v>
+        <v>1.41</v>
       </c>
       <c r="Z12" t="n">
-        <v>2.5</v>
+        <v>2.62</v>
       </c>
       <c r="AA12" t="n">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="AB12" t="n">
-        <v>1.3</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Troyes</t>
+          <t>Bayer Leverkusen</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Rodez</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="C13" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="K13" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="P13" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="R13" t="n">
+        <v>7</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="T13" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="U13" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="V13" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="W13" t="n">
+        <v>3</v>
+      </c>
+      <c r="X13" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Westerlo</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Dender</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="K14" t="n">
+        <v>4</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="P14" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="R14" t="n">
+        <v>5</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="T14" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="U14" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="V14" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="W14" t="n">
+        <v>4</v>
+      </c>
+      <c r="X14" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Raith</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Ayr</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="I15" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="R15" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="S15" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="U15" t="n">
+        <v>4</v>
+      </c>
+      <c r="V15" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="W15" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="X15" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>West Brom</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="K16" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="P16" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="R16" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="T16" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="U16" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="V16" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="W16" t="n">
+        <v>6</v>
+      </c>
+      <c r="X16" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Lille</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Lyon</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="I17" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="K17" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="P17" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="R17" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="T17" t="n">
         <v>2.3</v>
       </c>
-      <c r="D13" t="n">
+      <c r="U17" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="V17" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="W17" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="X17" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Alaves</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Mallorca</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="K18" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="O18" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="R18" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="S18" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="T18" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="U18" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="V18" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="W18" t="n">
+        <v>13</v>
+      </c>
+      <c r="X18" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Sporting CP</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Estrela</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="D19" t="n">
+        <v>11</v>
+      </c>
+      <c r="E19" t="n">
+        <v>23</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="H19" t="n">
+        <v>8</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="J19" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K19" t="n">
+        <v>15</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="N19" t="n">
+        <v>3</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="R19" t="n">
+        <v>8</v>
+      </c>
+      <c r="S19" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="T19" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="U19" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="V19" t="n">
+        <v>2</v>
+      </c>
+      <c r="W19" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="X19" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Central Cordoba</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="I20" t="n">
         <v>3.25</v>
       </c>
-      <c r="E13" t="n">
-        <v>2.88</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="G13" t="n">
+      <c r="J20" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="K20" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="N20" t="n">
         <v>1.33</v>
       </c>
-      <c r="H13" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="I13" t="n">
+      <c r="O20" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="R20" t="n">
+        <v>2</v>
+      </c>
+      <c r="S20" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="T20" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U20" t="n">
+        <v>8</v>
+      </c>
+      <c r="V20" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="W20" t="n">
+        <v>19</v>
+      </c>
+      <c r="X20" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Gimnasia L.P.</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="D21" t="n">
         <v>3</v>
       </c>
-      <c r="J13" t="n">
+      <c r="E21" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="I21" t="n">
+        <v>3</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="K21" t="n">
+        <v>5</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="O21" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P21" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="R21" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="S21" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="T21" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="U21" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V21" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="W21" t="n">
+        <v>17</v>
+      </c>
+      <c r="X21" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="Z21" t="n">
         <v>2.1</v>
       </c>
-      <c r="K13" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="L13" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="M13" t="n">
-        <v>1.67</v>
-      </c>
-      <c r="N13" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="O13" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="P13" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="R13" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="S13" t="n">
-        <v>1.98</v>
-      </c>
-      <c r="T13" t="n">
-        <v>1.88</v>
-      </c>
-      <c r="U13" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="V13" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="W13" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="X13" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>1.36</v>
+      <c r="AA21" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>